<commit_message>
Stack Pointer Implemented, All Source Modules updated for RAT Computer
</commit_message>
<xml_diff>
--- a/RAT TestCaseNotes.xlsx
+++ b/RAT TestCaseNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisg\Desktop\Winter 2018\CPE-233\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B6B23C-D2E5-45E0-87A2-8D2D31E31E1F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB828662-B3C3-49CD-A45A-4AB521B1B90F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13290" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phase1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="61">
   <si>
     <t>Expected Out</t>
   </si>
@@ -186,20 +186,32 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>Fail</t>
-  </si>
-  <si>
     <t>Test fixed by commeting out Data .DB 1</t>
   </si>
   <si>
-    <t>RST pauses the count down</t>
+    <t>SSEG</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>XXX0</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>R-&gt;L slowly, no reset?</t>
+  </si>
+  <si>
+    <t>1…7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -214,8 +226,14 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,6 +243,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEFEFEF"/>
+        <bgColor rgb="FFEFEFEF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFEFEFEF"/>
       </patternFill>
     </fill>
@@ -241,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -252,6 +276,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,16 +596,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z8"/>
+  <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.5703125" customWidth="1"/>
     <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.28515625" bestFit="1" customWidth="1"/>
@@ -603,6 +630,9 @@
       <c r="F1" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="2" t="s">
@@ -621,7 +651,9 @@
       <c r="F2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -658,6 +690,9 @@
       <c r="F3" t="s">
         <v>53</v>
       </c>
+      <c r="G3" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" s="2" t="s">
@@ -676,7 +711,9 @@
       <c r="F4" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -711,7 +748,10 @@
         <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="G5" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:26">
@@ -727,13 +767,15 @@
       <c r="D6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>56</v>
+      <c r="E6" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -768,18 +810,42 @@
         <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F7" t="s">
         <v>53</v>
       </c>
+      <c r="G7" s="7" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" s="4"/>
     </row>
+    <row r="9" spans="1:26" ht="15" customHeight="1">
+      <c r="A9" s="4"/>
+    </row>
+    <row r="10" spans="1:26" ht="15" customHeight="1">
+      <c r="A10" s="4"/>
+    </row>
+    <row r="11" spans="1:26" ht="15" customHeight="1">
+      <c r="A11" s="4"/>
+    </row>
+    <row r="12" spans="1:26" ht="15" customHeight="1">
+      <c r="A12" s="4"/>
+    </row>
+    <row r="13" spans="1:26" ht="15" customHeight="1">
+      <c r="A13" s="4"/>
+    </row>
+    <row r="14" spans="1:26" ht="15" customHeight="1">
+      <c r="A14" s="4"/>
+    </row>
+    <row r="15" spans="1:26" ht="15" customHeight="1">
+      <c r="A15" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -790,15 +856,20 @@
   </sheetPr>
   <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8.7109375" customWidth="1"/>
     <col min="2" max="2" width="48.85546875" customWidth="1"/>
-    <col min="3" max="3" width="43.42578125" customWidth="1"/>
-    <col min="4" max="4" width="29.140625" customWidth="1"/>
-    <col min="5" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -815,8 +886,12 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -851,8 +926,12 @@
         <v>16</v>
       </c>
       <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -886,6 +965,12 @@
       <c r="D3" t="s">
         <v>27</v>
       </c>
+      <c r="F3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" s="2" t="s">
@@ -901,8 +986,12 @@
         <v>30</v>
       </c>
       <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -936,6 +1025,12 @@
       <c r="D5" t="s">
         <v>30</v>
       </c>
+      <c r="F5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="6" spans="1:26">
       <c r="A6" s="2" t="s">
@@ -951,8 +1046,12 @@
         <v>43</v>
       </c>
       <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -986,6 +1085,12 @@
       <c r="D7" t="s">
         <v>41</v>
       </c>
+      <c r="F7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" s="3" t="s">
@@ -995,8 +1100,12 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>

</xml_diff>